<commit_message>
testing python file and results in xlsx
</commit_message>
<xml_diff>
--- a/translated_words.xlsx
+++ b/translated_words.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,82 +424,154 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Iegarena</t>
+          <t>English Word</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Latvian Translation</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tendrils</t>
+          <t>elongated</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Iegarena</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lodveida kopas</t>
+          <t>tendrils</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tendrils</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>plūdmaiņu straumes</t>
+          <t>globular clusters</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lodveida kopas</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tuvā infrasarkanā kamera</t>
+          <t>tidal streams</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>plūdmaiņu straumes</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tumšā matērija</t>
+          <t>near-infrared camera</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tuvā infrasarkanā kamera</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>liela mēroga struktūra</t>
+          <t>dark matter</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>tumšā matērija</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gadījumos</t>
+          <t>large-scale structure</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>liela mēroga struktūra</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>viela</t>
+          <t>instances</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gadījumos</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>deflācija</t>
+          <t>substance</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>viela</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Oļi</t>
+          <t>deflating</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>deflācija</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
+        <is>
+          <t>pebbles</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Oļi</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>hematite</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>hematīts</t>
         </is>

</xml_diff>